<commit_message>
Products in backend working perfectly
</commit_message>
<xml_diff>
--- a/app/Recursos Marcas/Molú/Plantilla modificada.xlsx
+++ b/app/Recursos Marcas/Molú/Plantilla modificada.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="124">
   <si>
     <t>Referencia</t>
   </si>
@@ -56,42 +56,6 @@
   </si>
   <si>
     <t>Color 6</t>
-  </si>
-  <si>
-    <t>Unnamed: 14</t>
-  </si>
-  <si>
-    <t>Unnamed: 15</t>
-  </si>
-  <si>
-    <t>Unnamed: 16</t>
-  </si>
-  <si>
-    <t>Unnamed: 17</t>
-  </si>
-  <si>
-    <t>Unnamed: 18</t>
-  </si>
-  <si>
-    <t>Unnamed: 19</t>
-  </si>
-  <si>
-    <t>Unnamed: 20</t>
-  </si>
-  <si>
-    <t>Unnamed: 21</t>
-  </si>
-  <si>
-    <t>Unnamed: 22</t>
-  </si>
-  <si>
-    <t>Unnamed: 23</t>
-  </si>
-  <si>
-    <t>Unnamed: 24</t>
-  </si>
-  <si>
-    <t>Unnamed: 25</t>
   </si>
   <si>
     <t>Imágenes</t>
@@ -431,7 +395,7 @@
     <t>['https://recursosmolova.s3.amazonaws.com/Products+Images/Molú/Cushy+Terra/Cushy+Terra+1+Naranja.png', 'https://recursosmolova.s3.amazonaws.com/Products+Images/Molú/Cushy+Terra/Cushy+Terra+2+Naranja.png', 'https://recursosmolova.s3.amazonaws.com/Products+Images/Molú/Cushy+Terra/Cushy+Terra+3+Naranja.png', 'https://recursosmolova.s3.amazonaws.com/Products+Images/Molú/Cushy+Terra/Cushy+Terra+4+Naranja.png']</t>
   </si>
   <si>
-    <t>['https://recursosmolova.s3.amazonaws.com/Products+Images/Molú/C%C2%A0rdigan+Montanhas/Cardigan+Montanhas+1.png', 'https://recursosmolova.s3.amazonaws.com/Products+Images/Molú/C%C2%A0rdigan+Montanhas/Cardigan+Montanhas+2.png', 'https://recursosmolova.s3.amazonaws.com/Products+Images/Molú/C%C2%A0rdigan+Montanhas/Cardigan+Montanhas+3.png', 'https://recursosmolova.s3.amazonaws.com/Products+Images/Molú/C%C2%A0rdigan+Montanhas/Cardigan+Montanhas+4.png', 'https://recursosmolova.s3.amazonaws.com/Products+Images/Molú/C%C2%A0rdigan+Montanhas/Cardigan+Montanhas+5.png', 'https://recursosmolova.s3.amazonaws.com/Products+Images/Molú/C%C2%A0rdigan+Montanhas/Cardigan+Montanhas+6.png']</t>
+    <t>['https://recursosmolova.s3.amazonaws.com/Products+Images/Molú/Ca%CC%81rdigan+Montanhas/Cardigan+Montanhas+1.png', 'https://recursosmolova.s3.amazonaws.com/Products+Images/Molú/Ca%CC%81rdigan+Montanhas/Cardigan+Montanhas+2.png', 'https://recursosmolova.s3.amazonaws.com/Products+Images/Molú/Ca%CC%81rdigan+Montanhas/Cardigan+Montanhas+3.png', 'https://recursosmolova.s3.amazonaws.com/Products+Images/Molú/Ca%CC%81rdigan+Montanhas/Cardigan+Montanhas+4.png', 'https://recursosmolova.s3.amazonaws.com/Products+Images/Molú/Ca%CC%81rdigan+Montanhas/Cardigan+Montanhas+5.png', 'https://recursosmolova.s3.amazonaws.com/Products+Images/Molú/Ca%CC%81rdigan+Montanhas/Cardigan+Montanhas+6.png']</t>
   </si>
   <si>
     <t>['https://recursosmolova.s3.amazonaws.com/Products+Images/Molú/Snug+Culotte/Snug+Culotte+1+Negro.png', 'https://recursosmolova.s3.amazonaws.com/Products+Images/Molú/Snug+Culotte/Snug+Culotte+2+Marron.png', 'https://recursosmolova.s3.amazonaws.com/Products+Images/Molú/Snug+Culotte/Snug+Culotte+3+Marron.png', 'https://recursosmolova.s3.amazonaws.com/Products+Images/Molú/Snug+Culotte/Snug+Culotte+4+Verde.png', 'https://recursosmolova.s3.amazonaws.com/Products+Images/Molú/Snug+Culotte/Snug+Culotte+5+Verde.png']</t>
@@ -814,13 +778,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AA20"/>
+  <dimension ref="A1:O20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:27">
+    <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -866,652 +830,616 @@
       <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:27">
-      <c r="A2" t="s">
-        <v>27</v>
-      </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="D2">
         <v>340000</v>
       </c>
       <c r="F2" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="G2" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="I2" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="J2" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="K2" t="s">
-        <v>113</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="3" spans="1:27">
+        <v>101</v>
+      </c>
+      <c r="O2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="D3">
         <v>330000</v>
       </c>
       <c r="F3" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="G3" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="I3" t="s">
-        <v>111</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="4" spans="1:27">
+        <v>99</v>
+      </c>
+      <c r="O3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="C4" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="D4">
         <v>325000</v>
       </c>
       <c r="F4" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="G4" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="I4" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="J4" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="K4" t="s">
-        <v>113</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27">
+        <v>101</v>
+      </c>
+      <c r="O4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="C5" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="D5">
         <v>170000</v>
       </c>
       <c r="F5" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="G5" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="I5" t="s">
-        <v>113</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="6" spans="1:27">
+        <v>101</v>
+      </c>
+      <c r="O5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="C6" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="D6">
         <v>170000</v>
       </c>
       <c r="F6" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="G6" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="I6" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="J6" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="K6" t="s">
-        <v>111</v>
-      </c>
-      <c r="AA6" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="7" spans="1:27">
+        <v>99</v>
+      </c>
+      <c r="O6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="C7" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="D7">
         <v>245000</v>
       </c>
       <c r="F7" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="G7" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="I7" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="J7" t="s">
+        <v>98</v>
+      </c>
+      <c r="K7" t="s">
+        <v>99</v>
+      </c>
+      <c r="L7" t="s">
+        <v>104</v>
+      </c>
+      <c r="O7" t="s">
         <v>110</v>
       </c>
-      <c r="K7" t="s">
-        <v>111</v>
-      </c>
-      <c r="L7" t="s">
-        <v>116</v>
-      </c>
-      <c r="AA7" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="8" spans="1:27">
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="C8" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="D8">
         <v>180000</v>
       </c>
       <c r="F8" t="s">
+        <v>73</v>
+      </c>
+      <c r="G8" t="s">
+        <v>76</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="G8" t="s">
-        <v>88</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>97</v>
-      </c>
       <c r="I8" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="J8" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="K8" t="s">
+        <v>99</v>
+      </c>
+      <c r="L8" t="s">
+        <v>98</v>
+      </c>
+      <c r="O8" t="s">
         <v>111</v>
       </c>
-      <c r="L8" t="s">
-        <v>110</v>
-      </c>
-      <c r="AA8" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="9" spans="1:27">
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="C9" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="D9">
         <v>195000</v>
       </c>
       <c r="F9" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="G9" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="H9" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="I9" t="s">
         <v>98</v>
       </c>
-      <c r="I9" t="s">
-        <v>110</v>
-      </c>
       <c r="J9" t="s">
+        <v>100</v>
+      </c>
+      <c r="K9" t="s">
+        <v>101</v>
+      </c>
+      <c r="L9" t="s">
+        <v>104</v>
+      </c>
+      <c r="O9" t="s">
         <v>112</v>
       </c>
-      <c r="K9" t="s">
-        <v>113</v>
-      </c>
-      <c r="L9" t="s">
-        <v>116</v>
-      </c>
-      <c r="AA9" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="10" spans="1:27">
+    </row>
+    <row r="10" spans="1:15">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="C10" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="D10">
         <v>190000</v>
       </c>
       <c r="F10" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="G10" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="I10" t="s">
-        <v>112</v>
-      </c>
-      <c r="AA10" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="11" spans="1:27">
+        <v>100</v>
+      </c>
+      <c r="O10" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="C11" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="D11">
         <v>205000</v>
       </c>
       <c r="F11" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="G11" t="s">
+        <v>76</v>
+      </c>
+      <c r="H11" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="H11" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="AA11" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="12" spans="1:27">
+      <c r="O11" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="B12" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="C12" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="D12">
         <v>205000</v>
       </c>
       <c r="F12" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="G12" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="I12" t="s">
-        <v>112</v>
-      </c>
-      <c r="AA12" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="13" spans="1:27">
+        <v>100</v>
+      </c>
+      <c r="O12" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="B13" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="C13" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="D13">
         <v>215000</v>
       </c>
       <c r="F13" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="G13" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="AA13" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="14" spans="1:27">
+        <v>90</v>
+      </c>
+      <c r="O13" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
       <c r="A14" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="B14" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C14" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="D14">
         <v>175000</v>
       </c>
       <c r="F14" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="G14" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="I14" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="J14" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="K14" t="s">
-        <v>116</v>
-      </c>
-      <c r="AA14" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="15" spans="1:27">
+        <v>104</v>
+      </c>
+      <c r="O14" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
       <c r="A15" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="C15" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="D15">
         <v>190000</v>
       </c>
       <c r="F15" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="G15" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="I15" t="s">
-        <v>114</v>
-      </c>
-      <c r="AA15" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="16" spans="1:27">
+        <v>102</v>
+      </c>
+      <c r="O15" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
       <c r="A16" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B16" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="C16" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="D16">
         <v>215000</v>
       </c>
       <c r="F16" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="G16" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="AA16" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="17" spans="1:27">
+        <v>93</v>
+      </c>
+      <c r="O16" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
       <c r="A17" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="B17" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="C17" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="D17">
         <v>160000</v>
       </c>
       <c r="F17" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="G17" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="I17" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="J17" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="K17" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="L17" t="s">
-        <v>110</v>
-      </c>
-      <c r="AA17" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="18" spans="1:27">
+        <v>98</v>
+      </c>
+      <c r="O17" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
       <c r="A18" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="B18" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="C18" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="D18">
         <v>175000</v>
       </c>
       <c r="F18" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="G18" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="I18" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="J18" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="K18" t="s">
-        <v>113</v>
-      </c>
-      <c r="AA18" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="19" spans="1:27">
+        <v>101</v>
+      </c>
+      <c r="O18" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
       <c r="A19" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="B19" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="C19" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="D19">
         <v>225000</v>
       </c>
       <c r="F19" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="G19" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="I19" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="J19" t="s">
-        <v>110</v>
-      </c>
-      <c r="AA19" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="20" spans="1:27">
+        <v>98</v>
+      </c>
+      <c r="O19" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15">
       <c r="A20" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="B20" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="C20" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="D20">
         <v>240000</v>
       </c>
       <c r="F20" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="G20" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="I20" t="s">
-        <v>115</v>
-      </c>
-      <c r="AA20" t="s">
-        <v>135</v>
+        <v>103</v>
+      </c>
+      <c r="O20" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>